<commit_message>
updating with latest changes for dev
</commit_message>
<xml_diff>
--- a/0.1.1/observations-summary.xlsx
+++ b/0.1.1/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="72">
   <si>
     <t>Profile</t>
   </si>
@@ -168,6 +168,27 @@
   </si>
   <si>
     <t>LOINC#882-1</t>
+  </si>
+  <si>
+    <t>ms-cmvgroup-observation</t>
+  </si>
+  <si>
+    <t>MSCmvObservation</t>
+  </si>
+  <si>
+    <t>LOINC#13949-3</t>
+  </si>
+  <si>
+    <t>ms-form117-observation</t>
+  </si>
+  <si>
+    <t>MSForm117Observation</t>
+  </si>
+  <si>
+    <t>[not stated]#FORM117COMPLIANCE</t>
+  </si>
+  <si>
+    <t>Quantity, CodeableConcept, string, boolean, integer, Range, Ratio, SampledData, time, dateTime, Period</t>
   </si>
   <si>
     <t>ms-height-observation</t>
@@ -340,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2559,22 +2580,22 @@
         <v>53</v>
       </c>
       <c r="C64" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D64" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E64" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="D64" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E64" t="s" s="2">
-        <v>55</v>
-      </c>
       <c r="F64" t="s" s="2">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="H64" t="s" s="2">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="I64" t="s" s="2">
         <v>18</v>
@@ -2588,10 +2609,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C65" t="s" s="2">
         <v>14</v>
@@ -2600,7 +2621,7 @@
         <v>14</v>
       </c>
       <c r="E65" t="s" s="2">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F65" t="s" s="2">
         <v>14</v>
@@ -2609,7 +2630,7 @@
         <v>16</v>
       </c>
       <c r="H65" t="s" s="2">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="I65" t="s" s="2">
         <v>18</v>
@@ -2623,28 +2644,28 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="B66" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="C66" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="D66" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E66" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="B66" t="s" s="2">
+      <c r="F66" t="s" s="2">
         <v>63</v>
       </c>
-      <c r="C66" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="D66" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E66" t="s" s="2">
+      <c r="G66" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="F66" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G66" t="s" s="2">
-        <v>57</v>
-      </c>
       <c r="H66" t="s" s="2">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I66" t="s" s="2">
         <v>18</v>
@@ -2653,6 +2674,76 @@
         <v>14</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="C67" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D67" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E67" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="F67" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G67" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="I67" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J67" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K67" t="s" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="B68" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="D68" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="F68" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="G68" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="H68" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="I68" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="J68" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>14</v>
       </c>
     </row>

</xml_diff>